<commit_message>
full cancelation and renewal
</commit_message>
<xml_diff>
--- a/Pathway/Pathwayusercredtinals.xlsx
+++ b/Pathway/Pathwayusercredtinals.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{544B2C0F-58BA-499E-ADB0-7030A7C2BC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BB56A5D2-A6FA-4974-B44C-29FE5D36CB64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="23304" windowHeight="13224" xr2:uid="{DEE4EFFF-2ED3-4D26-BD22-5CBBE4A017EA}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23280" windowHeight="13224" xr2:uid="{DEE4EFFF-2ED3-4D26-BD22-5CBBE4A017EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>